<commit_message>
Changed PU resistor to 1KOhm
</commit_message>
<xml_diff>
--- a/PCB/SoilSensorBOM.xlsx
+++ b/PCB/SoilSensorBOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20384"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S290244\Desktop\SoilSensor\PCB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/s290244_studenti_polito_it/Documents/Innovative wireless platforms for the internet of things/SoilSensor/PCB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{5E4DCED2-7E5A-49C8-95AB-EDDB58643A4F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:40009_{5E4DCED2-7E5A-49C8-95AB-EDDB58643A4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{642D758E-9659-4083-B517-99B01AC2D451}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13380"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="23040" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SOILSCHEMATIC" sheetId="1" r:id="rId1"/>
@@ -79,9 +79,6 @@
     <t>R1,R2</t>
   </si>
   <si>
-    <t>5k</t>
-  </si>
-  <si>
     <t>U1</t>
   </si>
   <si>
@@ -173,12 +170,15 @@
   </si>
   <si>
     <t>Thin Film Resistors - SMD 1/8W 5Kohms 0.05% 5ppm</t>
+  </si>
+  <si>
+    <t>1k</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -665,54 +665,54 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="20% - Colore 1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Colore 2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Colore 3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Colore 4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Colore 5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Colore 6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Colore 1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Colore 2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Colore 3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Colore 4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Colore 5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Colore 6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Colore 1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Colore 2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Colore 3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Colore 4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Colore 5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Colore 6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Calcolo" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Cella collegata" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Cella da controllare" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Colore 1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Colore 2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Colore 3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Colore 4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Colore 5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Colore 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Neutrale" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Nota" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Testo avviso" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Testo descrittivo" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Titolo" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Titolo 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Titolo 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Titolo 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Titolo 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Totale" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Valore non valido" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Valore valido" xfId="6" builtinId="26" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -728,7 +728,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1023,11 +1023,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1070,24 +1070,24 @@
         <v>6</v>
       </c>
       <c r="E12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" t="s">
         <v>23</v>
       </c>
-      <c r="F12" t="s">
-        <v>24</v>
-      </c>
       <c r="G12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
@@ -1102,14 +1102,14 @@
       <c r="D15" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" t="s">
         <v>25</v>
       </c>
-      <c r="F15" t="s">
-        <v>26</v>
-      </c>
       <c r="G15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -1126,13 +1126,13 @@
         <v>11</v>
       </c>
       <c r="E16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" t="s">
         <v>41</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>42</v>
-      </c>
-      <c r="G16" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -1149,13 +1149,13 @@
         <v>13</v>
       </c>
       <c r="E17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" t="s">
         <v>27</v>
       </c>
-      <c r="F17" t="s">
-        <v>28</v>
-      </c>
       <c r="G17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -1172,13 +1172,13 @@
         <v>15</v>
       </c>
       <c r="E18" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" t="s">
         <v>46</v>
       </c>
-      <c r="F18" t="s">
-        <v>47</v>
-      </c>
       <c r="G18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -1195,13 +1195,13 @@
         <v>17</v>
       </c>
       <c r="E19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" t="s">
         <v>37</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>38</v>
-      </c>
-      <c r="G19" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -1215,16 +1215,16 @@
         <v>18</v>
       </c>
       <c r="D20" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="E20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" t="s">
         <v>48</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>49</v>
-      </c>
-      <c r="G20" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -1235,19 +1235,19 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E21" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" t="s">
         <v>29</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>30</v>
-      </c>
-      <c r="G21" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -1258,19 +1258,19 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" t="s">
         <v>21</v>
       </c>
-      <c r="D22" t="s">
-        <v>22</v>
-      </c>
       <c r="E22" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" t="s">
         <v>34</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>35</v>
-      </c>
-      <c r="G22" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added testpoints on PCB, removed rendundant ones
</commit_message>
<xml_diff>
--- a/PCB/SoilSensorBOM.xlsx
+++ b/PCB/SoilSensorBOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/s290244_studenti_polito_it/Documents/Innovative wireless platforms for the internet of things/SoilSensor/PCB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:40009_{5E4DCED2-7E5A-49C8-95AB-EDDB58643A4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{642D758E-9659-4083-B517-99B01AC2D451}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{518F81A9-C8A4-4EAA-8D74-8C1B46E57007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="1920" windowWidth="23040" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>Soil Moisture Sensor  Revised: Wednesday, March 30, 2022</t>
   </si>
@@ -49,9 +49,6 @@
     <t>C2</t>
   </si>
   <si>
-    <t>33p</t>
-  </si>
-  <si>
     <t>C3,C6</t>
   </si>
   <si>
@@ -94,12 +91,6 @@
     <t>Prod ID</t>
   </si>
   <si>
-    <t>581-08055C330JAT2A</t>
-  </si>
-  <si>
-    <t>08055C330JAT2A</t>
-  </si>
-  <si>
     <t>581-08055C104M</t>
   </si>
   <si>
@@ -151,9 +142,6 @@
     <t>Condensatori in ceramica multistrato MLCC - SMD/SMT 50V 1uF X7R 0805 20%</t>
   </si>
   <si>
-    <t>Condensatori in ceramica multistrato MLCC - SMD/SMT 50V 33pF X7R 0805 5%</t>
-  </si>
-  <si>
     <t>Terminali e capicorda 4 POS RECPT R/A HV-190</t>
   </si>
   <si>
@@ -163,16 +151,43 @@
     <t>87995-4</t>
   </si>
   <si>
-    <t>71-TNPU08055K00AZEN0</t>
-  </si>
-  <si>
-    <t>TNPU08055K00AZEN00</t>
-  </si>
-  <si>
-    <t>Thin Film Resistors - SMD 1/8W 5Kohms 0.05% 5ppm</t>
-  </si>
-  <si>
     <t>1k</t>
+  </si>
+  <si>
+    <t>3.3p</t>
+  </si>
+  <si>
+    <t>TP1,TP2,TP3,TP4</t>
+  </si>
+  <si>
+    <t>TEST POINT</t>
+  </si>
+  <si>
+    <t>581-08055C3R3KAT2A</t>
+  </si>
+  <si>
+    <t>08055C3R3KAT2A</t>
+  </si>
+  <si>
+    <t>Condensatori in ceramica multistrato MLCC - SMD/SMT T101 COMMERCIAL</t>
+  </si>
+  <si>
+    <t>667-ERJ-6GEYJ102V</t>
+  </si>
+  <si>
+    <t>ERJ-6GEYJ102V</t>
+  </si>
+  <si>
+    <t>Resistori a pellicola spessa - SMD 0805 1Kohms 5% AEC-Q200</t>
+  </si>
+  <si>
+    <t>279-RCS-0C</t>
+  </si>
+  <si>
+    <t>RCS-0C</t>
+  </si>
+  <si>
+    <t>Resistori a strato metallico - SMD CIRC PROBE PAD</t>
   </si>
 </sst>
 </file>
@@ -663,12 +678,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Colore 1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1024,10 +1040,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1070,13 +1086,13 @@
         <v>6</v>
       </c>
       <c r="E12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" t="s">
         <v>22</v>
       </c>
-      <c r="F12" t="s">
-        <v>23</v>
-      </c>
       <c r="G12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -1100,16 +1116,16 @@
         <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="F15" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="G15" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -1120,19 +1136,19 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" t="s">
         <v>10</v>
       </c>
-      <c r="D16" t="s">
-        <v>11</v>
-      </c>
       <c r="E16" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F16" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G16" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -1143,19 +1159,19 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" t="s">
         <v>12</v>
       </c>
-      <c r="D17" t="s">
-        <v>13</v>
-      </c>
       <c r="E17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F17" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G17" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -1166,19 +1182,19 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" t="s">
         <v>14</v>
       </c>
-      <c r="D18" t="s">
-        <v>15</v>
-      </c>
       <c r="E18" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F18" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G18" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -1189,19 +1205,19 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" t="s">
         <v>16</v>
       </c>
-      <c r="D19" t="s">
-        <v>17</v>
-      </c>
       <c r="E19" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G19" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -1212,19 +1228,19 @@
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" t="s">
         <v>50</v>
       </c>
-      <c r="E20" t="s">
-        <v>47</v>
-      </c>
       <c r="F20" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G20" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -1235,19 +1251,19 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D21" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F21" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G21" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -1258,19 +1274,42 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" t="s">
         <v>20</v>
       </c>
-      <c r="D22" t="s">
-        <v>21</v>
-      </c>
       <c r="E22" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F22" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G22" t="s">
-        <v>35</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>9</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" t="s">
+        <v>53</v>
+      </c>
+      <c r="F23" t="s">
+        <v>54</v>
+      </c>
+      <c r="G23" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>